<commit_message>
fixing dataset and analysis
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morvaridrahbar/Desktop/Spell_corection/persian_Spell_Correction-_for_non-native/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morvaridrahbar/Desktop/Data correction/persian_Spell_Correction-_for_non-native/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDFEC2E-F034-3E44-975C-5B7E2F91C62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D969A7-0D35-C045-8F0E-18FD1667B450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8303,7 +8303,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8610,7 +8610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2571"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2542" zoomScale="109" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
       <selection activeCell="B2390" sqref="B2390:D2390"/>
     </sheetView>
   </sheetViews>

</xml_diff>